<commit_message>
updated the excel empty rows
</commit_message>
<xml_diff>
--- a/CS 230 CA EXCEL SHEET.xlsx
+++ b/CS 230 CA EXCEL SHEET.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="358">
   <si>
     <t>NAME</t>
   </si>
@@ -311,6 +311,9 @@
     <t>21164180</t>
   </si>
   <si>
+    <t>O</t>
+  </si>
+  <si>
     <t>EMMANUEL BWALYA</t>
   </si>
   <si>
@@ -525,6 +528,9 @@
   </si>
   <si>
     <t>22175822</t>
+  </si>
+  <si>
+    <t>A0</t>
   </si>
   <si>
     <t>LEO MABUKU</t>
@@ -2308,7 +2314,7 @@
   <dimension ref="A1:L173"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+      <selection activeCell="I173" sqref="I173"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -2374,7 +2380,9 @@
         <f t="shared" ref="G2:G26" si="0">15+3</f>
         <v>18</v>
       </c>
-      <c r="H2" s="5"/>
+      <c r="H2" s="5">
+        <v>0</v>
+      </c>
       <c r="I2" s="4">
         <v>5</v>
       </c>
@@ -2406,9 +2414,15 @@
       <c r="E3" s="4">
         <v>25</v>
       </c>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
+      <c r="F3" s="4">
+        <v>0</v>
+      </c>
+      <c r="G3" s="4">
+        <v>0</v>
+      </c>
+      <c r="H3" s="4">
+        <v>0</v>
+      </c>
       <c r="I3" s="4">
         <v>4</v>
       </c>
@@ -2431,7 +2445,9 @@
       <c r="B4" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="7"/>
+      <c r="C4" s="7">
+        <v>0</v>
+      </c>
       <c r="D4" s="7">
         <v>40</v>
       </c>
@@ -2445,7 +2461,9 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="H4" s="7"/>
+      <c r="H4" s="7">
+        <v>0</v>
+      </c>
       <c r="I4" s="7">
         <v>4</v>
       </c>
@@ -2484,7 +2502,9 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="H5" s="4"/>
+      <c r="H5" s="4">
+        <v>0</v>
+      </c>
       <c r="I5" s="4">
         <v>4</v>
       </c>
@@ -2564,7 +2584,9 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="H7" s="4"/>
+      <c r="H7" s="4">
+        <v>0</v>
+      </c>
       <c r="I7" s="4">
         <v>5</v>
       </c>
@@ -2596,7 +2618,9 @@
       <c r="E8" s="4">
         <v>6</v>
       </c>
-      <c r="F8" s="4"/>
+      <c r="F8" s="4">
+        <v>0</v>
+      </c>
       <c r="G8" s="4">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -2642,8 +2666,12 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
+      <c r="H9" s="4">
+        <v>0</v>
+      </c>
+      <c r="I9" s="4">
+        <v>0</v>
+      </c>
       <c r="J9" s="4">
         <v>102</v>
       </c>
@@ -2720,7 +2748,9 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="H11" s="4"/>
+      <c r="H11" s="4">
+        <v>0</v>
+      </c>
       <c r="I11" s="4">
         <v>4</v>
       </c>
@@ -2759,8 +2789,12 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
+      <c r="H12" s="4">
+        <v>0</v>
+      </c>
+      <c r="I12" s="4">
+        <v>0</v>
+      </c>
       <c r="J12" s="4">
         <v>96</v>
       </c>
@@ -2796,7 +2830,9 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="H13" s="4"/>
+      <c r="H13" s="4">
+        <v>0</v>
+      </c>
       <c r="I13" s="4">
         <v>4</v>
       </c>
@@ -2876,7 +2912,9 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="H15" s="4"/>
+      <c r="H15" s="4">
+        <v>0</v>
+      </c>
       <c r="I15" s="4">
         <v>1</v>
       </c>
@@ -2915,8 +2953,12 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
+      <c r="H16" s="4">
+        <v>0</v>
+      </c>
+      <c r="I16" s="4">
+        <v>0</v>
+      </c>
       <c r="J16" s="4">
         <v>67</v>
       </c>
@@ -2993,8 +3035,12 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
+      <c r="H18" s="4">
+        <v>0</v>
+      </c>
+      <c r="I18" s="4">
+        <v>0</v>
+      </c>
       <c r="J18" s="4">
         <v>109</v>
       </c>
@@ -3030,8 +3076,12 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
+      <c r="H19" s="4">
+        <v>0</v>
+      </c>
+      <c r="I19" s="4">
+        <v>0</v>
+      </c>
       <c r="J19" s="4">
         <v>96</v>
       </c>
@@ -3067,8 +3117,12 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
+      <c r="H20" s="9">
+        <v>0</v>
+      </c>
+      <c r="I20" s="9">
+        <v>0</v>
+      </c>
       <c r="J20" s="9">
         <v>105</v>
       </c>
@@ -3097,12 +3151,16 @@
       <c r="E21" s="4">
         <v>13</v>
       </c>
-      <c r="F21" s="4"/>
+      <c r="F21" s="4">
+        <v>0</v>
+      </c>
       <c r="G21" s="4">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="H21" s="4"/>
+      <c r="H21" s="4">
+        <v>0</v>
+      </c>
       <c r="I21" s="4">
         <v>4</v>
       </c>
@@ -3131,14 +3189,22 @@
       <c r="D22" s="4">
         <v>71</v>
       </c>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
+      <c r="E22" s="4">
+        <v>0</v>
+      </c>
+      <c r="F22" s="4">
+        <v>0</v>
+      </c>
       <c r="G22" s="4">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
+      <c r="H22" s="4">
+        <v>0</v>
+      </c>
+      <c r="I22" s="4">
+        <v>0</v>
+      </c>
       <c r="J22" s="4">
         <v>100</v>
       </c>
@@ -3254,8 +3320,12 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="H25" s="4"/>
-      <c r="I25" s="4"/>
+      <c r="H25" s="4">
+        <v>0</v>
+      </c>
+      <c r="I25" s="4">
+        <v>0</v>
+      </c>
       <c r="J25" s="4">
         <v>71</v>
       </c>
@@ -3291,7 +3361,9 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="H26" s="4"/>
+      <c r="H26" s="4">
+        <v>0</v>
+      </c>
       <c r="I26" s="4">
         <v>5</v>
       </c>
@@ -3329,8 +3401,12 @@
       <c r="G27" s="7">
         <v>18</v>
       </c>
-      <c r="H27" s="7"/>
-      <c r="I27" s="7"/>
+      <c r="H27" s="7">
+        <v>0</v>
+      </c>
+      <c r="I27" s="7">
+        <v>0</v>
+      </c>
       <c r="J27" s="7">
         <v>57</v>
       </c>
@@ -3366,7 +3442,9 @@
         <f t="shared" ref="G28:G30" si="3">15+3</f>
         <v>18</v>
       </c>
-      <c r="H28" s="4"/>
+      <c r="H28" s="4">
+        <v>0</v>
+      </c>
       <c r="I28" s="4">
         <v>5</v>
       </c>
@@ -3446,7 +3524,9 @@
         <f t="shared" si="3"/>
         <v>18</v>
       </c>
-      <c r="H30" s="4"/>
+      <c r="H30" s="4">
+        <v>0</v>
+      </c>
       <c r="I30" s="4">
         <v>4</v>
       </c>
@@ -3481,10 +3561,18 @@
       <c r="F31" s="4">
         <v>20</v>
       </c>
-      <c r="G31" s="4"/>
-      <c r="H31" s="4"/>
-      <c r="I31" s="4"/>
-      <c r="J31" s="4"/>
+      <c r="G31" s="4">
+        <v>0</v>
+      </c>
+      <c r="H31" s="4">
+        <v>0</v>
+      </c>
+      <c r="I31" s="4">
+        <v>0</v>
+      </c>
+      <c r="J31" s="4">
+        <v>0</v>
+      </c>
       <c r="K31" s="10">
         <f t="shared" si="1"/>
         <v>18.695652173913</v>
@@ -3559,7 +3647,9 @@
       <c r="H33" s="4">
         <v>9</v>
       </c>
-      <c r="I33" s="4"/>
+      <c r="I33" s="4">
+        <v>0</v>
+      </c>
       <c r="J33" s="4">
         <v>53</v>
       </c>
@@ -3591,11 +3681,15 @@
       <c r="F34" s="4">
         <v>11</v>
       </c>
-      <c r="G34" s="4"/>
+      <c r="G34" s="4">
+        <v>0</v>
+      </c>
       <c r="H34" s="4">
         <v>13</v>
       </c>
-      <c r="I34" s="4"/>
+      <c r="I34" s="4">
+        <v>0</v>
+      </c>
       <c r="J34" s="4">
         <v>75</v>
       </c>
@@ -3631,7 +3725,9 @@
         <f t="shared" si="4"/>
         <v>18</v>
       </c>
-      <c r="H35" s="4"/>
+      <c r="H35" s="4">
+        <v>0</v>
+      </c>
       <c r="I35" s="4">
         <v>4</v>
       </c>
@@ -3668,7 +3764,9 @@
         <f t="shared" si="4"/>
         <v>18</v>
       </c>
-      <c r="H36" s="4"/>
+      <c r="H36" s="4">
+        <v>0</v>
+      </c>
       <c r="I36" s="4">
         <v>3</v>
       </c>
@@ -3703,7 +3801,9 @@
       <c r="F37" s="4">
         <v>25</v>
       </c>
-      <c r="G37" s="4"/>
+      <c r="G37" s="4">
+        <v>0</v>
+      </c>
       <c r="H37" s="4">
         <v>11</v>
       </c>
@@ -3786,7 +3886,9 @@
         <f t="shared" si="5"/>
         <v>18</v>
       </c>
-      <c r="H39" s="4"/>
+      <c r="H39" s="4">
+        <v>0</v>
+      </c>
       <c r="I39" s="4">
         <v>4</v>
       </c>
@@ -3821,8 +3923,12 @@
       <c r="F40" s="4">
         <v>19</v>
       </c>
-      <c r="G40" s="4"/>
-      <c r="H40" s="4"/>
+      <c r="G40" s="4">
+        <v>0</v>
+      </c>
+      <c r="H40" s="4">
+        <v>0</v>
+      </c>
       <c r="I40" s="4">
         <v>4</v>
       </c>
@@ -3861,8 +3967,12 @@
         <f t="shared" si="5"/>
         <v>18</v>
       </c>
-      <c r="H41" s="4"/>
-      <c r="I41" s="4"/>
+      <c r="H41" s="4">
+        <v>0</v>
+      </c>
+      <c r="I41" s="4">
+        <v>0</v>
+      </c>
       <c r="J41" s="4">
         <v>170</v>
       </c>
@@ -3894,9 +4004,15 @@
       <c r="F42" s="9">
         <v>16</v>
       </c>
-      <c r="G42" s="9"/>
-      <c r="H42" s="9"/>
-      <c r="I42" s="9"/>
+      <c r="G42" s="9">
+        <v>0</v>
+      </c>
+      <c r="H42" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="I42" s="9">
+        <v>0</v>
+      </c>
       <c r="J42" s="9">
         <v>117</v>
       </c>
@@ -3911,10 +4027,10 @@
     </row>
     <row r="43" spans="1:12">
       <c r="A43" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B43" s="13" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C43" s="4">
         <v>28</v>
@@ -3928,10 +4044,18 @@
       <c r="F43" s="4">
         <v>17</v>
       </c>
-      <c r="G43" s="4"/>
-      <c r="H43" s="4"/>
-      <c r="I43" s="4"/>
-      <c r="J43" s="4"/>
+      <c r="G43" s="4">
+        <v>0</v>
+      </c>
+      <c r="H43" s="4">
+        <v>0</v>
+      </c>
+      <c r="I43" s="4">
+        <v>0</v>
+      </c>
+      <c r="J43" s="4">
+        <v>0</v>
+      </c>
       <c r="K43" s="10">
         <f t="shared" si="1"/>
         <v>25.2173913043478</v>
@@ -3943,10 +4067,10 @@
     </row>
     <row r="44" spans="1:12">
       <c r="A44" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B44" s="13" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C44" s="4">
         <v>20</v>
@@ -3984,10 +4108,10 @@
     </row>
     <row r="45" spans="1:12">
       <c r="A45" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B45" s="13" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C45" s="4">
         <v>20</v>
@@ -4005,7 +4129,9 @@
         <f t="shared" si="6"/>
         <v>18</v>
       </c>
-      <c r="H45" s="4"/>
+      <c r="H45" s="4">
+        <v>0</v>
+      </c>
       <c r="I45" s="4">
         <v>5</v>
       </c>
@@ -4023,10 +4149,10 @@
     </row>
     <row r="46" spans="1:12">
       <c r="A46" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B46" s="13" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C46" s="4">
         <v>34</v>
@@ -4040,9 +4166,15 @@
       <c r="F46" s="4">
         <v>21</v>
       </c>
-      <c r="G46" s="4"/>
-      <c r="H46" s="4"/>
-      <c r="I46" s="4"/>
+      <c r="G46" s="4">
+        <v>0</v>
+      </c>
+      <c r="H46" s="4">
+        <v>0</v>
+      </c>
+      <c r="I46" s="4">
+        <v>0</v>
+      </c>
       <c r="J46" s="4">
         <v>156</v>
       </c>
@@ -4057,10 +4189,10 @@
     </row>
     <row r="47" spans="1:12">
       <c r="A47" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B47" s="13" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C47" s="4">
         <v>43</v>
@@ -4098,10 +4230,10 @@
     </row>
     <row r="48" spans="1:12">
       <c r="A48" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B48" s="13" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C48" s="4">
         <v>35</v>
@@ -4119,7 +4251,9 @@
         <f t="shared" si="6"/>
         <v>18</v>
       </c>
-      <c r="H48" s="4"/>
+      <c r="H48" s="4">
+        <v>0</v>
+      </c>
       <c r="I48" s="4">
         <v>3</v>
       </c>
@@ -4137,10 +4271,10 @@
     </row>
     <row r="49" spans="1:12">
       <c r="A49" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B49" s="13" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C49" s="4">
         <v>17</v>
@@ -4161,7 +4295,9 @@
       <c r="H49" s="4">
         <v>10</v>
       </c>
-      <c r="I49" s="4"/>
+      <c r="I49" s="4">
+        <v>0</v>
+      </c>
       <c r="J49" s="4">
         <v>74</v>
       </c>
@@ -4176,10 +4312,10 @@
     </row>
     <row r="50" spans="1:12">
       <c r="A50" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B50" s="13" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C50" s="4">
         <v>7</v>
@@ -4193,9 +4329,15 @@
       <c r="F50" s="4">
         <v>13</v>
       </c>
-      <c r="G50" s="4"/>
-      <c r="H50" s="4"/>
-      <c r="I50" s="4"/>
+      <c r="G50" s="4">
+        <v>0</v>
+      </c>
+      <c r="H50" s="4">
+        <v>0</v>
+      </c>
+      <c r="I50" s="4">
+        <v>0</v>
+      </c>
       <c r="J50" s="4">
         <v>23</v>
       </c>
@@ -4210,10 +4352,10 @@
     </row>
     <row r="51" spans="1:12">
       <c r="A51" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B51" s="13" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C51" s="4">
         <v>26</v>
@@ -4231,8 +4373,12 @@
         <f t="shared" ref="G51:G60" si="7">15+3</f>
         <v>18</v>
       </c>
-      <c r="H51" s="4"/>
-      <c r="I51" s="4"/>
+      <c r="H51" s="4">
+        <v>0</v>
+      </c>
+      <c r="I51" s="4">
+        <v>0</v>
+      </c>
       <c r="J51" s="4">
         <v>119</v>
       </c>
@@ -4247,10 +4393,10 @@
     </row>
     <row r="52" spans="1:12">
       <c r="A52" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B52" s="13" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C52" s="4">
         <v>29</v>
@@ -4268,7 +4414,9 @@
         <f t="shared" si="7"/>
         <v>18</v>
       </c>
-      <c r="H52" s="4"/>
+      <c r="H52" s="4">
+        <v>9</v>
+      </c>
       <c r="I52" s="4">
         <v>3</v>
       </c>
@@ -4277,19 +4425,19 @@
       </c>
       <c r="K52" s="10">
         <f t="shared" si="1"/>
-        <v>55</v>
+        <v>56.9565217391304</v>
       </c>
       <c r="L52" s="10">
         <f t="shared" si="2"/>
-        <v>22</v>
+        <v>22.7826086956522</v>
       </c>
     </row>
     <row r="53" spans="1:12">
       <c r="A53" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B53" s="13" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C53" s="4">
         <v>27</v>
@@ -4303,8 +4451,12 @@
       <c r="F53" s="4">
         <v>17</v>
       </c>
-      <c r="G53" s="4"/>
-      <c r="H53" s="4"/>
+      <c r="G53" s="4">
+        <v>0</v>
+      </c>
+      <c r="H53" s="4">
+        <v>0</v>
+      </c>
       <c r="I53" s="4">
         <v>5</v>
       </c>
@@ -4322,10 +4474,10 @@
     </row>
     <row r="54" spans="1:12">
       <c r="A54" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B54" s="13" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C54" s="4">
         <v>29</v>
@@ -4336,10 +4488,18 @@
       <c r="E54" s="4">
         <v>15</v>
       </c>
-      <c r="F54" s="4"/>
-      <c r="G54" s="4"/>
-      <c r="H54" s="4"/>
-      <c r="I54" s="4"/>
+      <c r="F54" s="4">
+        <v>0</v>
+      </c>
+      <c r="G54" s="4">
+        <v>0</v>
+      </c>
+      <c r="H54" s="4">
+        <v>0</v>
+      </c>
+      <c r="I54" s="4">
+        <v>0</v>
+      </c>
       <c r="J54" s="4">
         <v>69</v>
       </c>
@@ -4354,10 +4514,10 @@
     </row>
     <row r="55" spans="1:12">
       <c r="A55" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B55" s="13" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C55" s="4">
         <v>32</v>
@@ -4375,8 +4535,12 @@
         <f t="shared" si="7"/>
         <v>18</v>
       </c>
-      <c r="H55" s="4"/>
-      <c r="I55" s="4"/>
+      <c r="H55" s="4">
+        <v>0</v>
+      </c>
+      <c r="I55" s="4">
+        <v>0</v>
+      </c>
       <c r="J55" s="4">
         <v>65</v>
       </c>
@@ -4391,10 +4555,10 @@
     </row>
     <row r="56" spans="1:12">
       <c r="A56" s="6" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B56" s="14" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C56" s="7">
         <v>37</v>
@@ -4432,10 +4596,10 @@
     </row>
     <row r="57" spans="1:12">
       <c r="A57" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B57" s="13" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C57" s="4">
         <v>25</v>
@@ -4453,11 +4617,15 @@
         <f t="shared" si="7"/>
         <v>18</v>
       </c>
-      <c r="H57" s="4"/>
+      <c r="H57" s="4">
+        <v>0</v>
+      </c>
       <c r="I57" s="4">
         <v>4</v>
       </c>
-      <c r="J57" s="4"/>
+      <c r="J57" s="4">
+        <v>0</v>
+      </c>
       <c r="K57" s="10">
         <f t="shared" si="1"/>
         <v>26.5217391304348</v>
@@ -4469,10 +4637,10 @@
     </row>
     <row r="58" spans="1:12">
       <c r="A58" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B58" s="13" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C58" s="4">
         <v>49</v>
@@ -4490,8 +4658,12 @@
         <f t="shared" si="7"/>
         <v>18</v>
       </c>
-      <c r="H58" s="4"/>
-      <c r="I58" s="4"/>
+      <c r="H58" s="4">
+        <v>0</v>
+      </c>
+      <c r="I58" s="4">
+        <v>0</v>
+      </c>
       <c r="J58" s="4">
         <v>108</v>
       </c>
@@ -4506,10 +4678,10 @@
     </row>
     <row r="59" spans="1:12">
       <c r="A59" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B59" s="13" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C59" s="4">
         <v>22</v>
@@ -4523,9 +4695,15 @@
         <f t="shared" si="7"/>
         <v>18</v>
       </c>
-      <c r="H59" s="4"/>
-      <c r="I59" s="4"/>
-      <c r="J59" s="4"/>
+      <c r="H59" s="4">
+        <v>0</v>
+      </c>
+      <c r="I59" s="4">
+        <v>0</v>
+      </c>
+      <c r="J59" s="4">
+        <v>0</v>
+      </c>
       <c r="K59" s="10">
         <f t="shared" si="1"/>
         <v>15.4347826086957</v>
@@ -4537,10 +4715,10 @@
     </row>
     <row r="60" spans="1:12">
       <c r="A60" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B60" s="13" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C60" s="4">
         <v>51</v>
@@ -4578,10 +4756,10 @@
     </row>
     <row r="61" spans="1:12">
       <c r="A61" s="6" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B61" s="14" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C61" s="7">
         <v>30</v>
@@ -4618,10 +4796,10 @@
     </row>
     <row r="62" spans="1:12">
       <c r="A62" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B62" s="13" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C62" s="4">
         <v>23</v>
@@ -4639,8 +4817,12 @@
         <f t="shared" ref="G62:G68" si="9">15+3</f>
         <v>18</v>
       </c>
-      <c r="H62" s="4"/>
-      <c r="I62" s="4"/>
+      <c r="H62" s="4">
+        <v>0</v>
+      </c>
+      <c r="I62" s="4">
+        <v>0</v>
+      </c>
       <c r="J62" s="4">
         <v>64</v>
       </c>
@@ -4655,10 +4837,10 @@
     </row>
     <row r="63" spans="1:12">
       <c r="A63" s="6" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B63" s="14" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C63" s="7">
         <v>16</v>
@@ -4675,8 +4857,12 @@
       <c r="G63" s="7">
         <v>18</v>
       </c>
-      <c r="H63" s="7"/>
-      <c r="I63" s="7"/>
+      <c r="H63" s="7">
+        <v>0</v>
+      </c>
+      <c r="I63" s="7">
+        <v>0</v>
+      </c>
       <c r="J63" s="7">
         <v>37</v>
       </c>
@@ -4691,10 +4877,10 @@
     </row>
     <row r="64" spans="1:12">
       <c r="A64" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B64" s="13" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C64" s="4">
         <v>25</v>
@@ -4712,7 +4898,9 @@
         <f t="shared" si="9"/>
         <v>18</v>
       </c>
-      <c r="H64" s="4"/>
+      <c r="H64" s="4">
+        <v>0</v>
+      </c>
       <c r="I64" s="4">
         <v>5</v>
       </c>
@@ -4730,10 +4918,10 @@
     </row>
     <row r="65" spans="1:12">
       <c r="A65" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B65" s="13" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C65" s="4">
         <v>30</v>
@@ -4771,10 +4959,10 @@
     </row>
     <row r="66" spans="1:12">
       <c r="A66" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B66" s="13" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C66" s="4">
         <v>33</v>
@@ -4792,8 +4980,12 @@
         <f t="shared" si="9"/>
         <v>18</v>
       </c>
-      <c r="H66" s="4"/>
-      <c r="I66" s="4"/>
+      <c r="H66" s="4">
+        <v>0</v>
+      </c>
+      <c r="I66" s="4">
+        <v>0</v>
+      </c>
       <c r="J66" s="4">
         <v>73</v>
       </c>
@@ -4808,10 +5000,10 @@
     </row>
     <row r="67" spans="1:12">
       <c r="A67" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B67" s="13" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C67" s="4">
         <v>32</v>
@@ -4829,7 +5021,9 @@
         <f t="shared" si="9"/>
         <v>18</v>
       </c>
-      <c r="H67" s="4"/>
+      <c r="H67" s="4">
+        <v>0</v>
+      </c>
       <c r="I67" s="4">
         <v>2</v>
       </c>
@@ -4847,10 +5041,10 @@
     </row>
     <row r="68" spans="1:12">
       <c r="A68" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B68" s="13" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C68" s="4">
         <v>11</v>
@@ -4868,8 +5062,12 @@
         <f t="shared" si="9"/>
         <v>18</v>
       </c>
-      <c r="H68" s="4"/>
-      <c r="I68" s="4"/>
+      <c r="H68" s="4">
+        <v>0</v>
+      </c>
+      <c r="I68" s="4">
+        <v>0</v>
+      </c>
       <c r="J68" s="4">
         <v>64</v>
       </c>
@@ -4884,10 +5082,10 @@
     </row>
     <row r="69" spans="1:12">
       <c r="A69" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B69" s="13" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C69" s="4">
         <v>32</v>
@@ -4902,8 +5100,12 @@
         <v>12</v>
       </c>
       <c r="G69" s="4"/>
-      <c r="H69" s="4"/>
-      <c r="I69" s="4"/>
+      <c r="H69" s="4">
+        <v>0</v>
+      </c>
+      <c r="I69" s="4">
+        <v>0</v>
+      </c>
       <c r="J69" s="4">
         <v>74</v>
       </c>
@@ -4918,10 +5120,10 @@
     </row>
     <row r="70" spans="1:12">
       <c r="A70" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B70" s="13" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C70" s="4">
         <v>20</v>
@@ -4959,10 +5161,10 @@
     </row>
     <row r="71" spans="1:12">
       <c r="A71" s="6" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B71" s="14" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C71" s="7">
         <v>31</v>
@@ -4973,10 +5175,18 @@
       <c r="E71" s="7">
         <v>25</v>
       </c>
-      <c r="F71" s="7"/>
-      <c r="G71" s="7"/>
-      <c r="H71" s="7"/>
-      <c r="I71" s="7"/>
+      <c r="F71" s="7">
+        <v>0</v>
+      </c>
+      <c r="G71" s="7">
+        <v>0</v>
+      </c>
+      <c r="H71" s="7">
+        <v>0</v>
+      </c>
+      <c r="I71" s="7">
+        <v>0</v>
+      </c>
       <c r="J71" s="7">
         <v>49</v>
       </c>
@@ -4991,10 +5201,10 @@
     </row>
     <row r="72" spans="1:12">
       <c r="A72" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B72" s="13" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C72" s="4">
         <v>36</v>
@@ -5012,7 +5222,9 @@
         <f t="shared" si="12"/>
         <v>18</v>
       </c>
-      <c r="H72" s="4"/>
+      <c r="H72" s="4">
+        <v>0</v>
+      </c>
       <c r="I72" s="4">
         <v>5</v>
       </c>
@@ -5030,10 +5242,10 @@
     </row>
     <row r="73" spans="1:12">
       <c r="A73" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B73" s="13" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C73" s="4">
         <v>25</v>
@@ -5051,8 +5263,12 @@
         <f t="shared" si="12"/>
         <v>18</v>
       </c>
-      <c r="H73" s="4"/>
-      <c r="I73" s="4"/>
+      <c r="H73" s="4">
+        <v>0</v>
+      </c>
+      <c r="I73" s="4">
+        <v>0</v>
+      </c>
       <c r="J73" s="4">
         <v>110</v>
       </c>
@@ -5067,10 +5283,10 @@
     </row>
     <row r="74" spans="1:12">
       <c r="A74" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B74" s="13" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C74" s="4">
         <v>29</v>
@@ -5084,8 +5300,12 @@
       <c r="F74" s="4">
         <v>19</v>
       </c>
-      <c r="G74" s="4"/>
-      <c r="H74" s="4"/>
+      <c r="G74" s="4">
+        <v>0</v>
+      </c>
+      <c r="H74" s="4">
+        <v>0</v>
+      </c>
       <c r="I74" s="4">
         <v>2</v>
       </c>
@@ -5103,10 +5323,10 @@
     </row>
     <row r="75" spans="1:12">
       <c r="A75" s="6" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B75" s="14" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C75" s="7">
         <v>38</v>
@@ -5123,8 +5343,12 @@
       <c r="G75" s="7">
         <v>18</v>
       </c>
-      <c r="H75" s="7"/>
-      <c r="I75" s="7"/>
+      <c r="H75" s="7">
+        <v>0</v>
+      </c>
+      <c r="I75" s="7">
+        <v>0</v>
+      </c>
       <c r="J75" s="7">
         <v>127</v>
       </c>
@@ -5139,10 +5363,10 @@
     </row>
     <row r="76" spans="1:12">
       <c r="A76" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B76" s="13" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C76" s="4">
         <v>39</v>
@@ -5160,7 +5384,9 @@
         <f t="shared" ref="G76:G79" si="13">15+3</f>
         <v>18</v>
       </c>
-      <c r="H76" s="4"/>
+      <c r="H76" s="4">
+        <v>0</v>
+      </c>
       <c r="I76" s="4">
         <v>5</v>
       </c>
@@ -5178,10 +5404,10 @@
     </row>
     <row r="77" spans="1:12">
       <c r="A77" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B77" s="13" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C77" s="4">
         <v>42</v>
@@ -5199,8 +5425,12 @@
         <f t="shared" si="13"/>
         <v>18</v>
       </c>
-      <c r="H77" s="4"/>
-      <c r="I77" s="4"/>
+      <c r="H77" s="4">
+        <v>0</v>
+      </c>
+      <c r="I77" s="4">
+        <v>0</v>
+      </c>
       <c r="J77" s="4">
         <v>104</v>
       </c>
@@ -5215,10 +5445,10 @@
     </row>
     <row r="78" spans="1:12">
       <c r="A78" s="1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B78" s="13" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C78" s="4">
         <v>27</v>
@@ -5230,29 +5460,35 @@
         <v>13</v>
       </c>
       <c r="F78" s="4">
-        <v>13</v>
-      </c>
-      <c r="G78" s="4"/>
-      <c r="H78" s="4"/>
-      <c r="I78" s="4"/>
+        <v>0</v>
+      </c>
+      <c r="G78" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="H78" s="4">
+        <v>0</v>
+      </c>
+      <c r="I78" s="4">
+        <v>0</v>
+      </c>
       <c r="J78" s="4">
         <v>33</v>
       </c>
       <c r="K78" s="10">
         <f t="shared" si="11"/>
-        <v>28.2608695652174</v>
+        <v>25.4347826086956</v>
       </c>
       <c r="L78" s="11">
         <f t="shared" si="10"/>
-        <v>11.304347826087</v>
+        <v>10.1739130434783</v>
       </c>
     </row>
     <row r="79" spans="1:12">
       <c r="A79" s="1" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B79" s="13" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C79" s="4">
         <v>34</v>
@@ -5263,7 +5499,9 @@
       <c r="E79" s="4">
         <v>6</v>
       </c>
-      <c r="F79" s="4"/>
+      <c r="F79" s="4">
+        <v>0</v>
+      </c>
       <c r="G79" s="4">
         <f t="shared" si="13"/>
         <v>18</v>
@@ -5288,10 +5526,10 @@
     </row>
     <row r="80" spans="1:12">
       <c r="A80" s="1" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B80" s="13" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="C80" s="4">
         <v>20</v>
@@ -5305,9 +5543,15 @@
       <c r="F80" s="4">
         <v>39</v>
       </c>
-      <c r="G80" s="4"/>
-      <c r="H80" s="4"/>
-      <c r="I80" s="4"/>
+      <c r="G80" s="4">
+        <v>0</v>
+      </c>
+      <c r="H80" s="4">
+        <v>0</v>
+      </c>
+      <c r="I80" s="4">
+        <v>0</v>
+      </c>
       <c r="J80" s="4">
         <v>33</v>
       </c>
@@ -5322,10 +5566,10 @@
     </row>
     <row r="81" spans="1:12">
       <c r="A81" s="8" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B81" s="15" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C81" s="9">
         <v>28</v>
@@ -5343,7 +5587,9 @@
         <f t="shared" ref="G81:G88" si="14">15+3</f>
         <v>18</v>
       </c>
-      <c r="H81" s="9"/>
+      <c r="H81" s="9">
+        <v>0</v>
+      </c>
       <c r="I81" s="9">
         <v>4</v>
       </c>
@@ -5361,10 +5607,10 @@
     </row>
     <row r="82" spans="1:12">
       <c r="A82" s="6" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B82" s="14" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C82" s="7">
         <v>35</v>
@@ -5381,8 +5627,12 @@
       <c r="G82" s="7">
         <v>18</v>
       </c>
-      <c r="H82" s="7"/>
-      <c r="I82" s="7"/>
+      <c r="H82" s="7">
+        <v>0</v>
+      </c>
+      <c r="I82" s="7">
+        <v>0</v>
+      </c>
       <c r="J82" s="7">
         <v>127</v>
       </c>
@@ -5397,10 +5647,10 @@
     </row>
     <row r="83" spans="1:12">
       <c r="A83" s="6" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B83" s="14" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C83" s="7">
         <v>48</v>
@@ -5438,10 +5688,10 @@
     </row>
     <row r="84" spans="1:12">
       <c r="A84" s="1" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B84" s="13" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C84" s="4">
         <v>23</v>
@@ -5449,7 +5699,9 @@
       <c r="D84" s="4">
         <v>23</v>
       </c>
-      <c r="E84" s="4"/>
+      <c r="E84" s="4">
+        <v>0</v>
+      </c>
       <c r="F84" s="4">
         <v>23</v>
       </c>
@@ -5457,8 +5709,12 @@
         <f t="shared" si="14"/>
         <v>18</v>
       </c>
-      <c r="H84" s="4"/>
-      <c r="I84" s="4"/>
+      <c r="H84" s="4">
+        <v>0</v>
+      </c>
+      <c r="I84" s="4">
+        <v>0</v>
+      </c>
       <c r="J84" s="4">
         <v>77</v>
       </c>
@@ -5473,10 +5729,10 @@
     </row>
     <row r="85" spans="1:12">
       <c r="A85" s="1" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B85" s="13" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C85" s="4">
         <v>31</v>
@@ -5494,7 +5750,9 @@
         <f t="shared" si="14"/>
         <v>18</v>
       </c>
-      <c r="H85" s="4"/>
+      <c r="H85" s="4">
+        <v>0</v>
+      </c>
       <c r="I85" s="4">
         <v>3</v>
       </c>
@@ -5512,10 +5770,10 @@
     </row>
     <row r="86" spans="1:12">
       <c r="A86" s="1" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B86" s="13" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C86" s="4">
         <v>43</v>
@@ -5533,7 +5791,9 @@
         <f t="shared" si="14"/>
         <v>18</v>
       </c>
-      <c r="H86" s="4"/>
+      <c r="H86" s="4">
+        <v>0</v>
+      </c>
       <c r="I86" s="4">
         <v>1</v>
       </c>
@@ -5551,10 +5811,10 @@
     </row>
     <row r="87" spans="1:12">
       <c r="A87" s="1" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B87" s="13" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="C87" s="4">
         <v>25</v>
@@ -5572,8 +5832,12 @@
         <f t="shared" si="14"/>
         <v>18</v>
       </c>
-      <c r="H87" s="4"/>
-      <c r="I87" s="4"/>
+      <c r="H87" s="4">
+        <v>0</v>
+      </c>
+      <c r="I87" s="4">
+        <v>0</v>
+      </c>
       <c r="J87" s="4">
         <v>128</v>
       </c>
@@ -5588,10 +5852,10 @@
     </row>
     <row r="88" spans="1:12">
       <c r="A88" s="1" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B88" s="13" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="C88" s="4">
         <v>34</v>
@@ -5629,10 +5893,10 @@
     </row>
     <row r="89" spans="1:12">
       <c r="A89" s="1" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B89" s="13" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="C89" s="4">
         <v>22</v>
@@ -5646,7 +5910,9 @@
       <c r="F89" s="4">
         <v>17</v>
       </c>
-      <c r="G89" s="4"/>
+      <c r="G89" s="4">
+        <v>0</v>
+      </c>
       <c r="H89" s="4">
         <v>4</v>
       </c>
@@ -5667,10 +5933,10 @@
     </row>
     <row r="90" spans="1:12">
       <c r="A90" s="1" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B90" s="13" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="C90" s="4">
         <v>17</v>
@@ -5684,9 +5950,15 @@
       <c r="F90" s="4">
         <v>11</v>
       </c>
-      <c r="G90" s="4"/>
-      <c r="H90" s="4"/>
-      <c r="I90" s="4"/>
+      <c r="G90" s="4">
+        <v>0</v>
+      </c>
+      <c r="H90" s="4">
+        <v>0</v>
+      </c>
+      <c r="I90" s="4">
+        <v>0</v>
+      </c>
       <c r="J90" s="4">
         <v>38</v>
       </c>
@@ -5701,10 +5973,10 @@
     </row>
     <row r="91" spans="1:12">
       <c r="A91" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B91" s="13" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="C91" s="7">
         <v>31</v>
@@ -5722,8 +5994,12 @@
         <f t="shared" ref="G91:G98" si="15">15+3</f>
         <v>18</v>
       </c>
-      <c r="H91" s="4"/>
-      <c r="I91" s="4"/>
+      <c r="H91" s="4">
+        <v>0</v>
+      </c>
+      <c r="I91" s="4">
+        <v>0</v>
+      </c>
       <c r="J91" s="4">
         <v>126</v>
       </c>
@@ -5738,10 +6014,10 @@
     </row>
     <row r="92" spans="1:12">
       <c r="A92" s="1" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B92" s="13" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="C92" s="4">
         <v>31</v>
@@ -5779,10 +6055,10 @@
     </row>
     <row r="93" spans="1:12">
       <c r="A93" s="8" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B93" s="15" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="C93" s="9">
         <v>34</v>
@@ -5800,8 +6076,12 @@
         <f t="shared" si="15"/>
         <v>18</v>
       </c>
-      <c r="H93" s="9"/>
-      <c r="I93" s="9"/>
+      <c r="H93" s="9">
+        <v>0</v>
+      </c>
+      <c r="I93" s="9">
+        <v>0</v>
+      </c>
       <c r="J93" s="9">
         <v>122</v>
       </c>
@@ -5816,10 +6096,10 @@
     </row>
     <row r="94" spans="1:12">
       <c r="A94" s="1" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="B94" s="13" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="C94" s="4">
         <v>20</v>
@@ -5837,7 +6117,9 @@
         <f t="shared" si="15"/>
         <v>18</v>
       </c>
-      <c r="H94" s="4"/>
+      <c r="H94" s="4">
+        <v>0</v>
+      </c>
       <c r="I94" s="4">
         <v>5</v>
       </c>
@@ -5855,10 +6137,10 @@
     </row>
     <row r="95" spans="1:12">
       <c r="A95" s="1" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B95" s="13" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="C95" s="4">
         <v>38</v>
@@ -5867,33 +6149,39 @@
         <v>22</v>
       </c>
       <c r="E95" s="4">
-        <v>20</v>
-      </c>
-      <c r="F95" s="4"/>
+        <v>0</v>
+      </c>
+      <c r="F95" s="4" t="s">
+        <v>167</v>
+      </c>
       <c r="G95" s="4">
         <f t="shared" si="15"/>
         <v>18</v>
       </c>
-      <c r="H95" s="4"/>
-      <c r="I95" s="4"/>
+      <c r="H95" s="4">
+        <v>0</v>
+      </c>
+      <c r="I95" s="4">
+        <v>0</v>
+      </c>
       <c r="J95" s="4">
         <v>107</v>
       </c>
       <c r="K95" s="10">
         <f t="shared" si="11"/>
-        <v>44.5652173913043</v>
+        <v>40.2173913043478</v>
       </c>
       <c r="L95" s="11">
         <f t="shared" si="10"/>
-        <v>17.8260869565217</v>
+        <v>16.0869565217391</v>
       </c>
     </row>
     <row r="96" spans="1:12">
       <c r="A96" s="1" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B96" s="13" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="C96" s="4">
         <v>33</v>
@@ -5911,7 +6199,9 @@
         <f t="shared" si="15"/>
         <v>18</v>
       </c>
-      <c r="H96" s="4"/>
+      <c r="H96" s="4">
+        <v>0</v>
+      </c>
       <c r="I96" s="4">
         <v>5</v>
       </c>
@@ -5929,10 +6219,10 @@
     </row>
     <row r="97" spans="1:12">
       <c r="A97" s="1" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B97" s="13" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="C97" s="4">
         <v>35</v>
@@ -5940,7 +6230,9 @@
       <c r="D97" s="4">
         <v>48</v>
       </c>
-      <c r="E97" s="4"/>
+      <c r="E97" s="4">
+        <v>0</v>
+      </c>
       <c r="F97" s="4">
         <v>19</v>
       </c>
@@ -5968,10 +6260,10 @@
     </row>
     <row r="98" spans="1:12">
       <c r="A98" s="1" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="B98" s="13" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="C98" s="4">
         <v>29</v>
@@ -6009,10 +6301,10 @@
     </row>
     <row r="99" spans="1:12">
       <c r="A99" s="1" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B99" s="13" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="C99" s="4">
         <v>17</v>
@@ -6020,14 +6312,24 @@
       <c r="D99" s="4">
         <v>29</v>
       </c>
-      <c r="E99" s="4"/>
-      <c r="F99" s="4"/>
-      <c r="G99" s="4"/>
-      <c r="H99" s="4"/>
+      <c r="E99" s="4">
+        <v>0</v>
+      </c>
+      <c r="F99" s="4">
+        <v>0</v>
+      </c>
+      <c r="G99" s="4">
+        <v>0</v>
+      </c>
+      <c r="H99" s="4">
+        <v>0</v>
+      </c>
       <c r="I99" s="4">
         <v>2</v>
       </c>
-      <c r="J99" s="4"/>
+      <c r="J99" s="4">
+        <v>0</v>
+      </c>
       <c r="K99" s="10">
         <f t="shared" si="11"/>
         <v>10.4347826086957</v>
@@ -6039,10 +6341,10 @@
     </row>
     <row r="100" spans="1:12">
       <c r="A100" s="6" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B100" s="14" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="C100" s="7">
         <v>33</v>
@@ -6056,7 +6358,9 @@
       <c r="F100" s="7">
         <v>17</v>
       </c>
-      <c r="G100" s="7"/>
+      <c r="G100" s="7">
+        <v>0</v>
+      </c>
       <c r="H100" s="7">
         <v>5</v>
       </c>
@@ -6077,10 +6381,10 @@
     </row>
     <row r="101" spans="1:12">
       <c r="A101" s="6" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B101" s="14" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="C101" s="7">
         <v>34</v>
@@ -6097,8 +6401,12 @@
       <c r="G101" s="7">
         <v>18</v>
       </c>
-      <c r="H101" s="7"/>
-      <c r="I101" s="7"/>
+      <c r="H101" s="7">
+        <v>0</v>
+      </c>
+      <c r="I101" s="7">
+        <v>0</v>
+      </c>
       <c r="J101" s="7">
         <v>138</v>
       </c>
@@ -6113,10 +6421,10 @@
     </row>
     <row r="102" spans="1:12">
       <c r="A102" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B102" s="13" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="C102" s="4">
         <v>21</v>
@@ -6132,8 +6440,12 @@
         <f t="shared" ref="G102:G104" si="16">15+3</f>
         <v>18</v>
       </c>
-      <c r="H102" s="4"/>
-      <c r="I102" s="4"/>
+      <c r="H102" s="4">
+        <v>0</v>
+      </c>
+      <c r="I102" s="4">
+        <v>0</v>
+      </c>
       <c r="J102" s="4">
         <v>127</v>
       </c>
@@ -6148,10 +6460,10 @@
     </row>
     <row r="103" spans="1:12">
       <c r="A103" s="1" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="B103" s="13" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="C103" s="4">
         <v>12</v>
@@ -6169,7 +6481,9 @@
         <f t="shared" si="16"/>
         <v>18</v>
       </c>
-      <c r="H103" s="4"/>
+      <c r="H103" s="4">
+        <v>0</v>
+      </c>
       <c r="I103" s="4">
         <v>1</v>
       </c>
@@ -6187,10 +6501,10 @@
     </row>
     <row r="104" spans="1:12">
       <c r="A104" s="1" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B104" s="13" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="C104" s="4">
         <v>37</v>
@@ -6201,12 +6515,16 @@
       <c r="E104" s="4">
         <v>16</v>
       </c>
-      <c r="F104" s="4"/>
+      <c r="F104" s="4">
+        <v>0</v>
+      </c>
       <c r="G104" s="4">
         <f t="shared" si="16"/>
         <v>18</v>
       </c>
-      <c r="H104" s="4"/>
+      <c r="H104" s="4">
+        <v>0</v>
+      </c>
       <c r="I104" s="4">
         <v>4</v>
       </c>
@@ -6224,10 +6542,10 @@
     </row>
     <row r="105" spans="1:12">
       <c r="A105" s="1" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="B105" s="13" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="C105" s="4">
         <v>29</v>
@@ -6241,11 +6559,15 @@
       <c r="F105" s="4">
         <v>23</v>
       </c>
-      <c r="G105" s="4"/>
+      <c r="G105" s="4">
+        <v>0</v>
+      </c>
       <c r="H105" s="4">
         <v>2</v>
       </c>
-      <c r="I105" s="4"/>
+      <c r="I105" s="4">
+        <v>0</v>
+      </c>
       <c r="J105" s="4">
         <v>75</v>
       </c>
@@ -6260,10 +6582,10 @@
     </row>
     <row r="106" spans="1:12">
       <c r="A106" s="1" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B106" s="13" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="C106" s="7">
         <v>33</v>
@@ -6281,8 +6603,12 @@
         <f t="shared" ref="G106:G108" si="17">15+3</f>
         <v>18</v>
       </c>
-      <c r="H106" s="4"/>
-      <c r="I106" s="4"/>
+      <c r="H106" s="4">
+        <v>0</v>
+      </c>
+      <c r="I106" s="4">
+        <v>0</v>
+      </c>
       <c r="J106" s="4">
         <v>166</v>
       </c>
@@ -6297,10 +6623,10 @@
     </row>
     <row r="107" spans="1:12">
       <c r="A107" s="1" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B107" s="13" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="C107" s="4">
         <v>29</v>
@@ -6338,10 +6664,10 @@
     </row>
     <row r="108" spans="1:12">
       <c r="A108" s="8" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="B108" s="15" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="C108" s="9">
         <v>39</v>
@@ -6359,8 +6685,12 @@
         <f t="shared" si="17"/>
         <v>18</v>
       </c>
-      <c r="H108" s="9"/>
-      <c r="I108" s="9"/>
+      <c r="H108" s="9">
+        <v>0</v>
+      </c>
+      <c r="I108" s="9">
+        <v>0</v>
+      </c>
       <c r="J108" s="9">
         <v>97</v>
       </c>
@@ -6375,10 +6705,10 @@
     </row>
     <row r="109" spans="1:12">
       <c r="A109" s="1" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="B109" s="13" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="C109" s="4">
         <v>33</v>
@@ -6392,9 +6722,15 @@
       <c r="F109" s="4">
         <v>11</v>
       </c>
-      <c r="G109" s="4"/>
-      <c r="H109" s="4"/>
-      <c r="I109" s="4"/>
+      <c r="G109" s="4">
+        <v>0</v>
+      </c>
+      <c r="H109" s="4">
+        <v>0</v>
+      </c>
+      <c r="I109" s="4">
+        <v>0</v>
+      </c>
       <c r="J109" s="4">
         <v>49</v>
       </c>
@@ -6409,10 +6745,10 @@
     </row>
     <row r="110" spans="1:12">
       <c r="A110" s="6" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="B110" s="14" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="C110" s="7">
         <v>34</v>
@@ -6450,10 +6786,10 @@
     </row>
     <row r="111" spans="1:12">
       <c r="A111" s="1" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="B111" s="13" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="C111" s="4">
         <v>43</v>
@@ -6471,7 +6807,9 @@
         <f t="shared" si="18"/>
         <v>18</v>
       </c>
-      <c r="H111" s="4"/>
+      <c r="H111" s="4">
+        <v>0</v>
+      </c>
       <c r="I111" s="4">
         <v>4</v>
       </c>
@@ -6489,10 +6827,10 @@
     </row>
     <row r="112" spans="1:12">
       <c r="A112" s="1" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="B112" s="13" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="C112" s="4">
         <v>23</v>
@@ -6510,7 +6848,9 @@
         <f t="shared" si="18"/>
         <v>18</v>
       </c>
-      <c r="H112" s="4"/>
+      <c r="H112" s="4">
+        <v>0</v>
+      </c>
       <c r="I112" s="4">
         <v>3</v>
       </c>
@@ -6528,10 +6868,10 @@
     </row>
     <row r="113" spans="1:12">
       <c r="A113" s="1" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="B113" s="13" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="C113" s="4">
         <v>29</v>
@@ -6549,7 +6889,9 @@
         <f t="shared" si="18"/>
         <v>18</v>
       </c>
-      <c r="H113" s="4"/>
+      <c r="H113" s="4">
+        <v>0</v>
+      </c>
       <c r="I113" s="4">
         <v>4</v>
       </c>
@@ -6567,10 +6909,10 @@
     </row>
     <row r="114" spans="1:12">
       <c r="A114" s="1" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="B114" s="13" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="C114" s="4">
         <v>13</v>
@@ -6588,8 +6930,12 @@
         <f t="shared" si="18"/>
         <v>18</v>
       </c>
-      <c r="H114" s="4"/>
-      <c r="I114" s="4"/>
+      <c r="H114" s="4">
+        <v>0</v>
+      </c>
+      <c r="I114" s="4">
+        <v>0</v>
+      </c>
       <c r="J114" s="4">
         <v>40</v>
       </c>
@@ -6604,10 +6950,10 @@
     </row>
     <row r="115" spans="1:12">
       <c r="A115" s="1" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="B115" s="13" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="C115" s="4">
         <v>30</v>
@@ -6616,10 +6962,18 @@
         <v>52</v>
       </c>
       <c r="E115" s="4"/>
-      <c r="F115" s="4"/>
-      <c r="G115" s="4"/>
-      <c r="H115" s="4"/>
-      <c r="I115" s="4"/>
+      <c r="F115" s="4">
+        <v>0</v>
+      </c>
+      <c r="G115" s="4">
+        <v>0</v>
+      </c>
+      <c r="H115" s="4">
+        <v>0</v>
+      </c>
+      <c r="I115" s="4">
+        <v>0</v>
+      </c>
       <c r="J115" s="4">
         <v>98</v>
       </c>
@@ -6634,10 +6988,10 @@
     </row>
     <row r="116" spans="1:12">
       <c r="A116" s="1" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="B116" s="13" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="C116" s="4">
         <v>37</v>
@@ -6648,13 +7002,19 @@
       <c r="E116" s="4">
         <v>16</v>
       </c>
-      <c r="F116" s="4"/>
+      <c r="F116" s="4">
+        <v>0</v>
+      </c>
       <c r="G116" s="4">
         <f t="shared" ref="G116:G119" si="19">15+3</f>
         <v>18</v>
       </c>
-      <c r="H116" s="4"/>
-      <c r="I116" s="4"/>
+      <c r="H116" s="4">
+        <v>0</v>
+      </c>
+      <c r="I116" s="4">
+        <v>0</v>
+      </c>
       <c r="J116" s="4">
         <v>87</v>
       </c>
@@ -6669,10 +7029,10 @@
     </row>
     <row r="117" spans="1:12">
       <c r="A117" s="1" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="B117" s="13" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="C117" s="4">
         <v>30</v>
@@ -6710,10 +7070,10 @@
     </row>
     <row r="118" spans="1:12">
       <c r="A118" s="1" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="B118" s="13" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="C118" s="4">
         <v>15</v>
@@ -6724,13 +7084,19 @@
       <c r="E118" s="4">
         <v>6</v>
       </c>
-      <c r="F118" s="4"/>
+      <c r="F118" s="4">
+        <v>0</v>
+      </c>
       <c r="G118" s="4">
         <f t="shared" si="19"/>
         <v>18</v>
       </c>
-      <c r="H118" s="4"/>
-      <c r="I118" s="4"/>
+      <c r="H118" s="4">
+        <v>0</v>
+      </c>
+      <c r="I118" s="4">
+        <v>0</v>
+      </c>
       <c r="J118" s="4">
         <v>38</v>
       </c>
@@ -6745,10 +7111,10 @@
     </row>
     <row r="119" spans="1:12">
       <c r="A119" s="1" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="B119" s="13" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="C119" s="4">
         <v>25</v>
@@ -6766,7 +7132,9 @@
         <f t="shared" si="19"/>
         <v>18</v>
       </c>
-      <c r="H119" s="4"/>
+      <c r="H119" s="4">
+        <v>0</v>
+      </c>
       <c r="I119" s="4">
         <v>2</v>
       </c>
@@ -6784,10 +7152,10 @@
     </row>
     <row r="120" spans="1:12">
       <c r="A120" s="8" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B120" s="15" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="C120" s="9">
         <v>18</v>
@@ -6798,10 +7166,18 @@
       <c r="E120" s="9">
         <v>3.5</v>
       </c>
-      <c r="F120" s="9"/>
-      <c r="G120" s="9"/>
-      <c r="H120" s="9"/>
-      <c r="I120" s="9"/>
+      <c r="F120" s="9">
+        <v>0</v>
+      </c>
+      <c r="G120" s="9">
+        <v>0</v>
+      </c>
+      <c r="H120" s="9">
+        <v>0</v>
+      </c>
+      <c r="I120" s="9">
+        <v>0</v>
+      </c>
       <c r="J120" s="9">
         <v>37</v>
       </c>
@@ -6816,10 +7192,10 @@
     </row>
     <row r="121" spans="1:12">
       <c r="A121" s="1" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="B121" s="13" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="C121" s="4">
         <v>29</v>
@@ -6837,7 +7213,9 @@
         <f t="shared" ref="G121:G133" si="20">15+3</f>
         <v>18</v>
       </c>
-      <c r="H121" s="4"/>
+      <c r="H121" s="4">
+        <v>0</v>
+      </c>
       <c r="I121" s="4">
         <v>4</v>
       </c>
@@ -6855,10 +7233,10 @@
     </row>
     <row r="122" spans="1:12">
       <c r="A122" s="1" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="B122" s="13" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="C122" s="4">
         <v>18</v>
@@ -6869,7 +7247,9 @@
       <c r="E122" s="4">
         <v>25</v>
       </c>
-      <c r="F122" s="4"/>
+      <c r="F122" s="4">
+        <v>0</v>
+      </c>
       <c r="G122" s="4">
         <f t="shared" si="20"/>
         <v>18</v>
@@ -6894,10 +7274,10 @@
     </row>
     <row r="123" spans="1:12">
       <c r="A123" s="1" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="B123" s="13" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="C123" s="4">
         <v>21</v>
@@ -6915,8 +7295,12 @@
         <f t="shared" si="20"/>
         <v>18</v>
       </c>
-      <c r="H123" s="4"/>
-      <c r="I123" s="4"/>
+      <c r="H123" s="4">
+        <v>0</v>
+      </c>
+      <c r="I123" s="4">
+        <v>0</v>
+      </c>
       <c r="J123" s="4">
         <v>86</v>
       </c>
@@ -6931,10 +7315,10 @@
     </row>
     <row r="124" spans="1:12">
       <c r="A124" s="1" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="B124" s="13" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="C124" s="4">
         <v>25</v>
@@ -6955,7 +7339,9 @@
       <c r="H124" s="4">
         <v>14</v>
       </c>
-      <c r="I124" s="4"/>
+      <c r="I124" s="4">
+        <v>0</v>
+      </c>
       <c r="J124" s="4">
         <v>107</v>
       </c>
@@ -6970,10 +7356,10 @@
     </row>
     <row r="125" spans="1:12">
       <c r="A125" s="1" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="B125" s="13" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="C125" s="4">
         <v>41</v>
@@ -6991,8 +7377,12 @@
         <f t="shared" si="20"/>
         <v>18</v>
       </c>
-      <c r="H125" s="4"/>
-      <c r="I125" s="4"/>
+      <c r="H125" s="4">
+        <v>0</v>
+      </c>
+      <c r="I125" s="4">
+        <v>0</v>
+      </c>
       <c r="J125" s="4">
         <v>141</v>
       </c>
@@ -7007,10 +7397,10 @@
     </row>
     <row r="126" spans="1:12">
       <c r="A126" s="1" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="B126" s="13" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="C126" s="4">
         <v>32</v>
@@ -7028,8 +7418,12 @@
         <f t="shared" si="20"/>
         <v>18</v>
       </c>
-      <c r="H126" s="4"/>
-      <c r="I126" s="4"/>
+      <c r="H126" s="4">
+        <v>0</v>
+      </c>
+      <c r="I126" s="4">
+        <v>0</v>
+      </c>
       <c r="J126" s="4">
         <v>88</v>
       </c>
@@ -7044,10 +7438,10 @@
     </row>
     <row r="127" spans="1:12">
       <c r="A127" s="1" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="B127" s="13" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="C127" s="4">
         <v>26</v>
@@ -7065,8 +7459,12 @@
         <f t="shared" si="20"/>
         <v>18</v>
       </c>
-      <c r="H127" s="4"/>
-      <c r="I127" s="4"/>
+      <c r="H127" s="4">
+        <v>0</v>
+      </c>
+      <c r="I127" s="4">
+        <v>0</v>
+      </c>
       <c r="J127" s="4">
         <v>136</v>
       </c>
@@ -7081,10 +7479,10 @@
     </row>
     <row r="128" spans="1:12">
       <c r="A128" s="8" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="B128" s="15" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="C128" s="4">
         <v>25</v>
@@ -7102,8 +7500,12 @@
         <f t="shared" si="20"/>
         <v>18</v>
       </c>
-      <c r="H128" s="4"/>
-      <c r="I128" s="4"/>
+      <c r="H128" s="4">
+        <v>0</v>
+      </c>
+      <c r="I128" s="4">
+        <v>0</v>
+      </c>
       <c r="J128" s="4">
         <v>95</v>
       </c>
@@ -7118,10 +7520,10 @@
     </row>
     <row r="129" spans="1:12">
       <c r="A129" s="1" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="B129" s="13" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="C129" s="4">
         <v>27</v>
@@ -7137,8 +7539,12 @@
         <f t="shared" si="20"/>
         <v>18</v>
       </c>
-      <c r="H129" s="4"/>
-      <c r="I129" s="4"/>
+      <c r="H129" s="4">
+        <v>0</v>
+      </c>
+      <c r="I129" s="4">
+        <v>0</v>
+      </c>
       <c r="J129" s="4">
         <v>58</v>
       </c>
@@ -7153,10 +7559,10 @@
     </row>
     <row r="130" spans="1:12">
       <c r="A130" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="B130" s="13" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="C130" s="4">
         <v>27</v>
@@ -7174,7 +7580,9 @@
         <f t="shared" si="20"/>
         <v>18</v>
       </c>
-      <c r="H130" s="4"/>
+      <c r="H130" s="4">
+        <v>0</v>
+      </c>
       <c r="I130" s="4">
         <v>3</v>
       </c>
@@ -7192,10 +7600,10 @@
     </row>
     <row r="131" spans="1:12">
       <c r="A131" s="1" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="B131" s="13" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="C131" s="4">
         <v>33</v>
@@ -7211,8 +7619,12 @@
         <f t="shared" si="20"/>
         <v>18</v>
       </c>
-      <c r="H131" s="4"/>
-      <c r="I131" s="4"/>
+      <c r="H131" s="4">
+        <v>0</v>
+      </c>
+      <c r="I131" s="4">
+        <v>0</v>
+      </c>
       <c r="J131" s="4">
         <v>56</v>
       </c>
@@ -7227,10 +7639,10 @@
     </row>
     <row r="132" spans="1:12">
       <c r="A132" s="1" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="B132" s="13" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C132" s="4">
         <v>24</v>
@@ -7248,8 +7660,12 @@
         <f t="shared" si="20"/>
         <v>18</v>
       </c>
-      <c r="H132" s="4"/>
-      <c r="I132" s="4"/>
+      <c r="H132" s="4">
+        <v>0</v>
+      </c>
+      <c r="I132" s="4">
+        <v>0</v>
+      </c>
       <c r="J132" s="4">
         <v>105</v>
       </c>
@@ -7264,10 +7680,10 @@
     </row>
     <row r="133" spans="1:12">
       <c r="A133" s="1" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="B133" s="13" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="C133" s="4">
         <v>25</v>
@@ -7285,7 +7701,9 @@
         <f t="shared" si="20"/>
         <v>18</v>
       </c>
-      <c r="H133" s="4"/>
+      <c r="H133" s="4">
+        <v>0</v>
+      </c>
       <c r="I133" s="4">
         <v>0</v>
       </c>
@@ -7303,10 +7721,10 @@
     </row>
     <row r="134" spans="1:12">
       <c r="A134" s="6" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="B134" s="14" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="C134" s="7">
         <v>17</v>
@@ -7323,7 +7741,9 @@
       <c r="G134" s="7">
         <v>18</v>
       </c>
-      <c r="H134" s="7"/>
+      <c r="H134" s="7">
+        <v>0</v>
+      </c>
       <c r="I134" s="7">
         <v>4</v>
       </c>
@@ -7341,10 +7761,10 @@
     </row>
     <row r="135" spans="1:12">
       <c r="A135" s="1" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="B135" s="13" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="C135" s="4">
         <v>56</v>
@@ -7362,7 +7782,9 @@
         <f t="shared" ref="G135:G138" si="23">15+3</f>
         <v>18</v>
       </c>
-      <c r="H135" s="4"/>
+      <c r="H135" s="4">
+        <v>0</v>
+      </c>
       <c r="I135" s="4">
         <v>5</v>
       </c>
@@ -7380,10 +7802,10 @@
     </row>
     <row r="136" spans="1:12">
       <c r="A136" s="1" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="B136" s="13" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="C136" s="4">
         <v>11</v>
@@ -7394,10 +7816,18 @@
       <c r="E136" s="4">
         <v>22</v>
       </c>
-      <c r="F136" s="4"/>
-      <c r="G136" s="4"/>
-      <c r="H136" s="4"/>
-      <c r="I136" s="4"/>
+      <c r="F136" s="4">
+        <v>0</v>
+      </c>
+      <c r="G136" s="4">
+        <v>0</v>
+      </c>
+      <c r="H136" s="4">
+        <v>0</v>
+      </c>
+      <c r="I136" s="4">
+        <v>0</v>
+      </c>
       <c r="J136" s="4">
         <v>81</v>
       </c>
@@ -7412,10 +7842,10 @@
     </row>
     <row r="137" spans="1:12">
       <c r="A137" s="1" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="B137" s="13" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="C137" s="4">
         <v>26</v>
@@ -7436,7 +7866,9 @@
       <c r="H137" s="4">
         <v>9</v>
       </c>
-      <c r="I137" s="4"/>
+      <c r="I137" s="4">
+        <v>0</v>
+      </c>
       <c r="J137" s="4">
         <v>93</v>
       </c>
@@ -7451,10 +7883,10 @@
     </row>
     <row r="138" spans="1:12">
       <c r="A138" s="1" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="B138" s="13" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="C138" s="4">
         <v>14</v>
@@ -7472,8 +7904,12 @@
         <f t="shared" si="23"/>
         <v>18</v>
       </c>
-      <c r="H138" s="4"/>
-      <c r="I138" s="4"/>
+      <c r="H138" s="4">
+        <v>0</v>
+      </c>
+      <c r="I138" s="4">
+        <v>0</v>
+      </c>
       <c r="J138" s="4">
         <v>55</v>
       </c>
@@ -7488,10 +7924,10 @@
     </row>
     <row r="139" spans="1:12">
       <c r="A139" s="1" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="B139" s="13" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="C139" s="4">
         <v>17</v>
@@ -7505,9 +7941,15 @@
       <c r="F139" s="4">
         <v>11</v>
       </c>
-      <c r="G139" s="4"/>
-      <c r="H139" s="4"/>
-      <c r="I139" s="4"/>
+      <c r="G139" s="4">
+        <v>0</v>
+      </c>
+      <c r="H139" s="4">
+        <v>0</v>
+      </c>
+      <c r="I139" s="4">
+        <v>0</v>
+      </c>
       <c r="J139" s="4">
         <v>45</v>
       </c>
@@ -7522,10 +7964,10 @@
     </row>
     <row r="140" spans="1:12">
       <c r="A140" s="1" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="B140" s="13" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="C140" s="4">
         <v>35</v>
@@ -7563,10 +8005,10 @@
     </row>
     <row r="141" spans="1:12">
       <c r="A141" s="6" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="B141" s="14" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="C141" s="7">
         <v>29</v>
@@ -7581,9 +8023,15 @@
       <c r="G141" s="7">
         <v>18</v>
       </c>
-      <c r="H141" s="7"/>
-      <c r="I141" s="7"/>
-      <c r="J141" s="7"/>
+      <c r="H141" s="7">
+        <v>0</v>
+      </c>
+      <c r="I141" s="7">
+        <v>0</v>
+      </c>
+      <c r="J141" s="7">
+        <v>0</v>
+      </c>
       <c r="K141" s="10">
         <f t="shared" si="22"/>
         <v>20.2173913043478</v>
@@ -7595,10 +8043,10 @@
     </row>
     <row r="142" spans="1:12">
       <c r="A142" s="1" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="B142" s="13" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="C142" s="4">
         <v>37</v>
@@ -7616,7 +8064,9 @@
         <f t="shared" si="24"/>
         <v>18</v>
       </c>
-      <c r="H142" s="4"/>
+      <c r="H142" s="4">
+        <v>0</v>
+      </c>
       <c r="I142" s="4">
         <v>5</v>
       </c>
@@ -7634,10 +8084,10 @@
     </row>
     <row r="143" spans="1:12">
       <c r="A143" s="1" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="B143" s="13" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="C143" s="4">
         <v>12</v>
@@ -7655,7 +8105,9 @@
         <f t="shared" si="24"/>
         <v>18</v>
       </c>
-      <c r="H143" s="4"/>
+      <c r="H143" s="4">
+        <v>0</v>
+      </c>
       <c r="I143" s="4">
         <v>0</v>
       </c>
@@ -7673,10 +8125,10 @@
     </row>
     <row r="144" spans="1:12">
       <c r="A144" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="B144" s="13" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="C144" s="4">
         <v>37</v>
@@ -7694,7 +8146,9 @@
         <f t="shared" si="24"/>
         <v>18</v>
       </c>
-      <c r="H144" s="4"/>
+      <c r="H144" s="4">
+        <v>0</v>
+      </c>
       <c r="I144" s="4">
         <v>5</v>
       </c>
@@ -7712,10 +8166,10 @@
     </row>
     <row r="145" spans="1:12">
       <c r="A145" s="1" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="B145" s="13" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="C145" s="4">
         <v>33</v>
@@ -7733,7 +8187,9 @@
         <f t="shared" si="24"/>
         <v>18</v>
       </c>
-      <c r="H145" s="4"/>
+      <c r="H145" s="4">
+        <v>0</v>
+      </c>
       <c r="I145" s="4">
         <v>5</v>
       </c>
@@ -7751,10 +8207,10 @@
     </row>
     <row r="146" spans="1:12">
       <c r="A146" s="1" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="B146" s="13" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="C146" s="4">
         <v>29</v>
@@ -7792,10 +8248,10 @@
     </row>
     <row r="147" spans="1:12">
       <c r="A147" s="1" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="B147" s="13" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="C147" s="4">
         <v>28</v>
@@ -7807,10 +8263,18 @@
       <c r="F147" s="4">
         <v>20</v>
       </c>
-      <c r="G147" s="4"/>
-      <c r="H147" s="4"/>
-      <c r="I147" s="4"/>
-      <c r="J147" s="4"/>
+      <c r="G147" s="4">
+        <v>0</v>
+      </c>
+      <c r="H147" s="4">
+        <v>0</v>
+      </c>
+      <c r="I147" s="4">
+        <v>0</v>
+      </c>
+      <c r="J147" s="4">
+        <v>0</v>
+      </c>
       <c r="K147" s="10">
         <f t="shared" si="22"/>
         <v>14.3478260869565</v>
@@ -7822,10 +8286,10 @@
     </row>
     <row r="148" spans="1:12">
       <c r="A148" s="1" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="B148" s="13" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="C148" s="4">
         <v>27</v>
@@ -7839,11 +8303,15 @@
       <c r="F148" s="4">
         <v>13</v>
       </c>
-      <c r="G148" s="4"/>
+      <c r="G148" s="4">
+        <v>0</v>
+      </c>
       <c r="H148" s="4">
         <v>10</v>
       </c>
-      <c r="I148" s="4"/>
+      <c r="I148" s="4">
+        <v>0</v>
+      </c>
       <c r="J148" s="4">
         <v>37</v>
       </c>
@@ -7858,10 +8326,10 @@
     </row>
     <row r="149" spans="1:12">
       <c r="A149" s="1" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="B149" s="13" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="C149" s="4">
         <v>38</v>
@@ -7879,8 +8347,12 @@
         <f t="shared" ref="G149:G157" si="25">15+3</f>
         <v>18</v>
       </c>
-      <c r="H149" s="4"/>
-      <c r="I149" s="4"/>
+      <c r="H149" s="4">
+        <v>0</v>
+      </c>
+      <c r="I149" s="4">
+        <v>0</v>
+      </c>
       <c r="J149" s="4">
         <v>68</v>
       </c>
@@ -7895,10 +8367,10 @@
     </row>
     <row r="150" spans="1:12">
       <c r="A150" s="1" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="B150" s="13" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="C150" s="4">
         <v>21</v>
@@ -7936,10 +8408,10 @@
     </row>
     <row r="151" spans="1:12">
       <c r="A151" s="1" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="B151" s="13" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="C151" s="4">
         <v>29</v>
@@ -7957,8 +8429,12 @@
         <f t="shared" si="25"/>
         <v>18</v>
       </c>
-      <c r="H151" s="4"/>
-      <c r="I151" s="4"/>
+      <c r="H151" s="4">
+        <v>0</v>
+      </c>
+      <c r="I151" s="4">
+        <v>0</v>
+      </c>
       <c r="J151" s="4">
         <v>75</v>
       </c>
@@ -7973,10 +8449,10 @@
     </row>
     <row r="152" spans="1:12">
       <c r="A152" s="1" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="B152" s="13" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="C152" s="4">
         <v>39</v>
@@ -7994,7 +8470,9 @@
         <f t="shared" si="25"/>
         <v>18</v>
       </c>
-      <c r="H152" s="4"/>
+      <c r="H152" s="4">
+        <v>0</v>
+      </c>
       <c r="I152" s="4">
         <v>5</v>
       </c>
@@ -8012,10 +8490,10 @@
     </row>
     <row r="153" spans="1:12">
       <c r="A153" s="1" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="B153" s="13" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="C153" s="4">
         <v>36</v>
@@ -8053,10 +8531,10 @@
     </row>
     <row r="154" spans="1:12">
       <c r="A154" s="1" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="B154" s="13" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="C154" s="4">
         <v>35</v>
@@ -8067,12 +8545,16 @@
       <c r="E154" s="4">
         <v>25</v>
       </c>
-      <c r="F154" s="4"/>
+      <c r="F154" s="4">
+        <v>0</v>
+      </c>
       <c r="G154" s="4">
         <f t="shared" si="25"/>
         <v>18</v>
       </c>
-      <c r="H154" s="4"/>
+      <c r="H154" s="4">
+        <v>0</v>
+      </c>
       <c r="I154" s="4">
         <v>3</v>
       </c>
@@ -8090,10 +8572,10 @@
     </row>
     <row r="155" spans="1:12">
       <c r="A155" s="1" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="B155" s="13" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="C155" s="4">
         <v>24</v>
@@ -8131,10 +8613,10 @@
     </row>
     <row r="156" spans="1:12">
       <c r="A156" s="1" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="B156" s="13" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="C156" s="4">
         <v>16</v>
@@ -8152,8 +8634,12 @@
         <f t="shared" si="25"/>
         <v>18</v>
       </c>
-      <c r="H156" s="4"/>
-      <c r="I156" s="4"/>
+      <c r="H156" s="4">
+        <v>0</v>
+      </c>
+      <c r="I156" s="4">
+        <v>0</v>
+      </c>
       <c r="J156" s="4">
         <v>49</v>
       </c>
@@ -8168,10 +8654,10 @@
     </row>
     <row r="157" spans="1:12">
       <c r="A157" s="1" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="B157" s="13" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="C157" s="4">
         <v>20</v>
@@ -8189,8 +8675,12 @@
         <f t="shared" si="25"/>
         <v>18</v>
       </c>
-      <c r="H157" s="4"/>
-      <c r="I157" s="4"/>
+      <c r="H157" s="4">
+        <v>0</v>
+      </c>
+      <c r="I157" s="4">
+        <v>0</v>
+      </c>
       <c r="J157" s="4">
         <v>74</v>
       </c>
@@ -8205,10 +8695,10 @@
     </row>
     <row r="158" spans="1:12">
       <c r="A158" s="1" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="B158" s="13" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="C158" s="4">
         <v>16</v>
@@ -8222,9 +8712,15 @@
       <c r="F158" s="4">
         <v>6</v>
       </c>
-      <c r="G158" s="4"/>
-      <c r="H158" s="4"/>
-      <c r="I158" s="4"/>
+      <c r="G158" s="4">
+        <v>0</v>
+      </c>
+      <c r="H158" s="4">
+        <v>0</v>
+      </c>
+      <c r="I158" s="4">
+        <v>0</v>
+      </c>
       <c r="J158" s="4">
         <v>101</v>
       </c>
@@ -8239,10 +8735,10 @@
     </row>
     <row r="159" spans="1:12">
       <c r="A159" s="1" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="B159" s="13" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="C159" s="4">
         <v>24</v>
@@ -8280,10 +8776,10 @@
     </row>
     <row r="160" spans="1:12">
       <c r="A160" s="1" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="B160" s="13" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="C160" s="4">
         <v>14</v>
@@ -8297,8 +8793,12 @@
       <c r="F160" s="4">
         <v>8</v>
       </c>
-      <c r="G160" s="4"/>
-      <c r="H160" s="4"/>
+      <c r="G160" s="4">
+        <v>0</v>
+      </c>
+      <c r="H160" s="4">
+        <v>0</v>
+      </c>
       <c r="I160" s="4">
         <v>1</v>
       </c>
@@ -8316,10 +8816,10 @@
     </row>
     <row r="161" spans="1:12">
       <c r="A161" s="1" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="B161" s="13" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="C161" s="4">
         <v>39</v>
@@ -8357,10 +8857,10 @@
     </row>
     <row r="162" spans="1:12">
       <c r="A162" s="6" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="B162" s="14" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="C162" s="7">
         <v>16</v>
@@ -8377,8 +8877,12 @@
       <c r="G162" s="7">
         <v>18</v>
       </c>
-      <c r="H162" s="7"/>
-      <c r="I162" s="7"/>
+      <c r="H162" s="7">
+        <v>0</v>
+      </c>
+      <c r="I162" s="7">
+        <v>0</v>
+      </c>
       <c r="J162" s="7">
         <v>39</v>
       </c>
@@ -8393,10 +8897,10 @@
     </row>
     <row r="163" spans="1:12">
       <c r="A163" s="1" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="B163" s="13" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="C163" s="4">
         <v>26</v>
@@ -8414,7 +8918,9 @@
         <f t="shared" si="26"/>
         <v>18</v>
       </c>
-      <c r="H163" s="4"/>
+      <c r="H163" s="4">
+        <v>0</v>
+      </c>
       <c r="I163" s="4">
         <v>5</v>
       </c>
@@ -8432,10 +8938,10 @@
     </row>
     <row r="164" spans="1:12">
       <c r="A164" s="1" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="B164" s="13" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="C164" s="4">
         <v>23</v>
@@ -8446,12 +8952,16 @@
       <c r="E164" s="4">
         <v>15</v>
       </c>
-      <c r="F164" s="4"/>
+      <c r="F164" s="4">
+        <v>0</v>
+      </c>
       <c r="G164" s="4">
         <f t="shared" si="26"/>
         <v>18</v>
       </c>
-      <c r="H164" s="4"/>
+      <c r="H164" s="4">
+        <v>0</v>
+      </c>
       <c r="I164" s="4">
         <v>4</v>
       </c>
@@ -8469,10 +8979,10 @@
     </row>
     <row r="165" spans="1:12">
       <c r="A165" s="1" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="B165" s="13" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="C165" s="4">
         <v>29</v>
@@ -8483,12 +8993,16 @@
       <c r="E165" s="4">
         <v>6</v>
       </c>
-      <c r="F165" s="4"/>
+      <c r="F165" s="4">
+        <v>0</v>
+      </c>
       <c r="G165" s="4">
         <f t="shared" si="26"/>
         <v>18</v>
       </c>
-      <c r="H165" s="4"/>
+      <c r="H165" s="4">
+        <v>0</v>
+      </c>
       <c r="I165" s="4"/>
       <c r="J165" s="4">
         <v>85</v>
@@ -8504,10 +9018,10 @@
     </row>
     <row r="166" spans="1:12">
       <c r="A166" s="1" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="B166" s="13" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="C166" s="4">
         <v>44</v>
@@ -8525,7 +9039,9 @@
         <f t="shared" si="26"/>
         <v>18</v>
       </c>
-      <c r="H166" s="4"/>
+      <c r="H166" s="4">
+        <v>0</v>
+      </c>
       <c r="I166" s="4">
         <v>5</v>
       </c>
@@ -8543,10 +9059,10 @@
     </row>
     <row r="167" spans="1:12">
       <c r="A167" s="6" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="B167" s="14" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="C167" s="7">
         <v>28</v>
@@ -8562,8 +9078,12 @@
         <f t="shared" si="26"/>
         <v>18</v>
       </c>
-      <c r="H167" s="7"/>
-      <c r="I167" s="7"/>
+      <c r="H167" s="7">
+        <v>0</v>
+      </c>
+      <c r="I167" s="7">
+        <v>0</v>
+      </c>
       <c r="J167" s="7">
         <v>65</v>
       </c>
@@ -8578,10 +9098,10 @@
     </row>
     <row r="168" spans="1:12">
       <c r="A168" s="1" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="B168" s="13" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="C168" s="4">
         <v>23</v>
@@ -8619,10 +9139,10 @@
     </row>
     <row r="169" spans="1:12">
       <c r="A169" s="1" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="B169" s="13" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="C169" s="4">
         <v>26</v>
@@ -8640,7 +9160,9 @@
         <f t="shared" si="26"/>
         <v>18</v>
       </c>
-      <c r="H169" s="4"/>
+      <c r="H169" s="4">
+        <v>0</v>
+      </c>
       <c r="I169" s="4">
         <v>5</v>
       </c>
@@ -8658,10 +9180,10 @@
     </row>
     <row r="170" spans="1:12">
       <c r="A170" s="1" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="B170" s="13" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="C170" s="4">
         <v>22</v>
@@ -8679,7 +9201,9 @@
         <f t="shared" si="26"/>
         <v>18</v>
       </c>
-      <c r="H170" s="4"/>
+      <c r="H170" s="4">
+        <v>0</v>
+      </c>
       <c r="I170" s="4">
         <v>4</v>
       </c>
@@ -8697,10 +9221,10 @@
     </row>
     <row r="171" spans="1:12">
       <c r="A171" s="1" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="B171" s="13" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="C171" s="4">
         <v>22</v>
@@ -8714,9 +9238,15 @@
       <c r="F171" s="4">
         <v>25</v>
       </c>
-      <c r="G171" s="4"/>
-      <c r="H171" s="4"/>
-      <c r="I171" s="4"/>
+      <c r="G171" s="4">
+        <v>0</v>
+      </c>
+      <c r="H171" s="4">
+        <v>0</v>
+      </c>
+      <c r="I171" s="4">
+        <v>0</v>
+      </c>
       <c r="J171" s="4">
         <v>63</v>
       </c>
@@ -8731,10 +9261,10 @@
     </row>
     <row r="172" spans="1:12">
       <c r="A172" s="1" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="B172" s="13" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="C172" s="4">
         <v>14</v>
@@ -8752,7 +9282,9 @@
         <f>15+3</f>
         <v>18</v>
       </c>
-      <c r="H172" s="4"/>
+      <c r="H172" s="4">
+        <v>0</v>
+      </c>
       <c r="I172" s="4">
         <v>1</v>
       </c>
@@ -8770,10 +9302,10 @@
     </row>
     <row r="173" spans="1:12">
       <c r="A173" s="1" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="B173" s="13" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="C173" s="4">
         <v>19</v>
@@ -8791,8 +9323,12 @@
         <f>15+3</f>
         <v>18</v>
       </c>
-      <c r="H173" s="4"/>
-      <c r="I173" s="4"/>
+      <c r="H173" s="4">
+        <v>0</v>
+      </c>
+      <c r="I173" s="4">
+        <v>0</v>
+      </c>
       <c r="J173" s="4">
         <v>62</v>
       </c>

</xml_diff>

<commit_message>
All the empty boxes in the excel sheet have been updated with a zero
</commit_message>
<xml_diff>
--- a/CS 230 CA EXCEL SHEET.xlsx
+++ b/CS 230 CA EXCEL SHEET.xlsx
@@ -2313,8 +2313,8 @@
   <sheetPr/>
   <dimension ref="A1:L173"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I173" sqref="I173"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G130" sqref="G130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -3274,7 +3274,9 @@
       <c r="E24" s="9">
         <v>13</v>
       </c>
-      <c r="F24" s="9"/>
+      <c r="F24" s="9">
+        <v>0</v>
+      </c>
       <c r="G24" s="4">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -3639,7 +3641,9 @@
       <c r="E33" s="4">
         <v>13</v>
       </c>
-      <c r="F33" s="4"/>
+      <c r="F33" s="4">
+        <v>0</v>
+      </c>
       <c r="G33" s="4">
         <f t="shared" si="4"/>
         <v>18</v>
@@ -3759,7 +3763,9 @@
       <c r="E36" s="4">
         <v>25</v>
       </c>
-      <c r="F36" s="4"/>
+      <c r="F36" s="4">
+        <v>0</v>
+      </c>
       <c r="G36" s="4">
         <f t="shared" si="4"/>
         <v>18</v>
@@ -4689,8 +4695,12 @@
       <c r="D59" s="4">
         <v>31</v>
       </c>
-      <c r="E59" s="4"/>
-      <c r="F59" s="4"/>
+      <c r="E59" s="4">
+        <v>0</v>
+      </c>
+      <c r="F59" s="4">
+        <v>0</v>
+      </c>
       <c r="G59" s="4">
         <f t="shared" si="7"/>
         <v>18</v>
@@ -5099,7 +5109,9 @@
       <c r="F69" s="4">
         <v>12</v>
       </c>
-      <c r="G69" s="4"/>
+      <c r="G69" s="4">
+        <v>0</v>
+      </c>
       <c r="H69" s="4">
         <v>0</v>
       </c>
@@ -6961,7 +6973,9 @@
       <c r="D115" s="4">
         <v>52</v>
       </c>
-      <c r="E115" s="4"/>
+      <c r="E115" s="4">
+        <v>0</v>
+      </c>
       <c r="F115" s="4">
         <v>0</v>
       </c>
@@ -7534,7 +7548,9 @@
       <c r="E129" s="4">
         <v>13</v>
       </c>
-      <c r="F129" s="4"/>
+      <c r="F129" s="4">
+        <v>0</v>
+      </c>
       <c r="G129" s="4">
         <f t="shared" si="20"/>
         <v>18</v>
@@ -7611,7 +7627,9 @@
       <c r="D131" s="4">
         <v>39</v>
       </c>
-      <c r="E131" s="4"/>
+      <c r="E131" s="4">
+        <v>0</v>
+      </c>
       <c r="F131" s="4">
         <v>13</v>
       </c>
@@ -8019,7 +8037,9 @@
       <c r="E141" s="7">
         <v>15</v>
       </c>
-      <c r="F141" s="7"/>
+      <c r="F141" s="7">
+        <v>0</v>
+      </c>
       <c r="G141" s="7">
         <v>18</v>
       </c>
@@ -8259,7 +8279,9 @@
       <c r="D147" s="4">
         <v>18</v>
       </c>
-      <c r="E147" s="4"/>
+      <c r="E147" s="4">
+        <v>0</v>
+      </c>
       <c r="F147" s="4">
         <v>20</v>
       </c>
@@ -9003,7 +9025,9 @@
       <c r="H165" s="4">
         <v>0</v>
       </c>
-      <c r="I165" s="4"/>
+      <c r="I165" s="4">
+        <v>0</v>
+      </c>
       <c r="J165" s="4">
         <v>85</v>
       </c>
@@ -9073,7 +9097,9 @@
       <c r="E167" s="7">
         <v>13</v>
       </c>
-      <c r="F167" s="7"/>
+      <c r="F167" s="7">
+        <v>0</v>
+      </c>
       <c r="G167" s="4">
         <f t="shared" si="26"/>
         <v>18</v>

</xml_diff>